<commit_message>
predicting for new data 20
</commit_message>
<xml_diff>
--- a/Kriging/Article/ExponentialModel/content/results/metrics_26_9.xlsx
+++ b/Kriging/Article/ExponentialModel/content/results/metrics_26_9.xlsx
@@ -518,661 +518,661 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_0</t>
+          <t>model_26_9_24</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9989305040943117</v>
+        <v>0.9975182599622946</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7963809470975685</v>
+        <v>0.6716090796131864</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9992815022415278</v>
+        <v>0.9952823018316802</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9985131344140157</v>
+        <v>0.9815534291385378</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9988586799717039</v>
+        <v>0.992625800406205</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0005319243094249506</v>
+        <v>0.00100038697235429</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1208770656879742</v>
+        <v>0.194947036090733</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0003180589480345667</v>
+        <v>0.002952246237628282</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0008808915557267374</v>
+        <v>0.003675796468756666</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0005994758314422818</v>
+        <v>0.003314026252657492</v>
       </c>
       <c r="L2" t="n">
-        <v>0.00709036010462986</v>
+        <v>0.004709588608930119</v>
       </c>
       <c r="M2" t="n">
-        <v>0.02306348432967037</v>
+        <v>0.0316288945800243</v>
       </c>
       <c r="N2" t="n">
-        <v>1.000634100031515</v>
+        <v>1.000677330796317</v>
       </c>
       <c r="O2" t="n">
-        <v>0.02317001369253412</v>
+        <v>0.03188294600726131</v>
       </c>
       <c r="P2" t="n">
-        <v>1181.078018708524</v>
+        <v>1179.814736762965</v>
       </c>
       <c r="Q2" t="n">
-        <v>3154.238640314562</v>
+        <v>2833.367088515676</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_1</t>
+          <t>model_26_9_23</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9990293828985012</v>
+        <v>0.9975380852147034</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7946737407971906</v>
+        <v>0.6715086549251414</v>
       </c>
       <c r="D3" t="n">
-        <v>0.999154741299458</v>
+        <v>0.9953258533788878</v>
       </c>
       <c r="E3" t="n">
-        <v>0.998449811009479</v>
+        <v>0.9816897684014174</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9987695578912537</v>
+        <v>0.9926863488841486</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0004827459634813281</v>
+        <v>0.0009923954325748708</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1218905370953508</v>
+        <v>0.1950066525236772</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0003741724868886134</v>
+        <v>0.002924992503540374</v>
       </c>
       <c r="J3" t="n">
-        <v>0.00091840742324163</v>
+        <v>0.003648628526009505</v>
       </c>
       <c r="K3" t="n">
-        <v>0.000646287007933693</v>
+        <v>0.003286815266175269</v>
       </c>
       <c r="L3" t="n">
-        <v>0.007659271136282723</v>
+        <v>0.004712475284367118</v>
       </c>
       <c r="M3" t="n">
-        <v>0.02197148068477243</v>
+        <v>0.03150230836898894</v>
       </c>
       <c r="N3" t="n">
-        <v>1.000575475166736</v>
+        <v>1.000671919974153</v>
       </c>
       <c r="O3" t="n">
-        <v>0.02207296612405235</v>
+        <v>0.03175534302317685</v>
       </c>
       <c r="P3" t="n">
-        <v>1181.2720399964</v>
+        <v>1179.830777817121</v>
       </c>
       <c r="Q3" t="n">
-        <v>3154.432661602439</v>
+        <v>2833.383129569833</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_2</t>
+          <t>model_26_9_22</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9990388298214075</v>
+        <v>0.9975597949208335</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7928270393050643</v>
+        <v>0.6713977041321872</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9989415581515044</v>
+        <v>0.9953727613465501</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9980889227335515</v>
+        <v>0.9818424356344664</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9984761884638247</v>
+        <v>0.9927528708599289</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0004780474434436291</v>
+        <v>0.0009836442713508731</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1229868188744277</v>
+        <v>0.1950725177071994</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0004685427294917121</v>
+        <v>0.002895638385047672</v>
       </c>
       <c r="J4" t="n">
-        <v>0.001132215206421201</v>
+        <v>0.00361820695441493</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0008003786536312262</v>
+        <v>0.003256919740388325</v>
       </c>
       <c r="L4" t="n">
-        <v>0.008253777267172559</v>
+        <v>0.004715788383673408</v>
       </c>
       <c r="M4" t="n">
-        <v>0.02186429608845501</v>
+        <v>0.03136310366259808</v>
       </c>
       <c r="N4" t="n">
-        <v>1.00056987412228</v>
+        <v>1.000665994836017</v>
       </c>
       <c r="O4" t="n">
-        <v>0.02196528644613359</v>
+        <v>0.03161502018873232</v>
       </c>
       <c r="P4" t="n">
-        <v>1181.291601152664</v>
+        <v>1179.848492478257</v>
       </c>
       <c r="Q4" t="n">
-        <v>3154.452222758703</v>
+        <v>2833.400844230968</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_3</t>
+          <t>model_26_9_21</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9990977635367797</v>
+        <v>0.9975847723161132</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7914184589026851</v>
+        <v>0.671267092698471</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9988317785264278</v>
+        <v>0.9954258006110998</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9980229556116464</v>
+        <v>0.9820219051179624</v>
       </c>
       <c r="F5" t="n">
-        <v>0.998392722726487</v>
+        <v>0.9928295709913497</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0004487361803667914</v>
+        <v>0.0009735759078391489</v>
       </c>
       <c r="H5" t="n">
-        <v>0.123823013048785</v>
+        <v>0.1951500542963736</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0005171391122302686</v>
+        <v>0.00286244741698936</v>
       </c>
       <c r="J5" t="n">
-        <v>0.001171297340804814</v>
+        <v>0.003582444573502048</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0008442188483591643</v>
+        <v>0.003222450067323766</v>
       </c>
       <c r="L5" t="n">
-        <v>0.008313823208062239</v>
+        <v>0.004718747327970767</v>
       </c>
       <c r="M5" t="n">
-        <v>0.02118339397657494</v>
+        <v>0.03120217793422678</v>
       </c>
       <c r="N5" t="n">
-        <v>1.000534932547866</v>
+        <v>1.000659177861323</v>
       </c>
       <c r="O5" t="n">
-        <v>0.02128123927312076</v>
+        <v>0.03145280186346458</v>
       </c>
       <c r="P5" t="n">
-        <v>1181.418150828952</v>
+        <v>1179.869069524075</v>
       </c>
       <c r="Q5" t="n">
-        <v>3154.578772434991</v>
+        <v>2833.421421276787</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_4</t>
+          <t>model_26_9_20</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9991209612088888</v>
+        <v>0.9976120826822439</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7903172401662691</v>
+        <v>0.67112375251888</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9987174295338507</v>
+        <v>0.9954846426636684</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9978634225137649</v>
+        <v>0.9822169256623632</v>
       </c>
       <c r="F6" t="n">
-        <v>0.998254568033097</v>
+        <v>0.9929137674100295</v>
       </c>
       <c r="G6" t="n">
-        <v>0.000437198589945653</v>
+        <v>0.0009625671260681696</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1244767440608941</v>
+        <v>0.1952351472189521</v>
       </c>
       <c r="I6" t="n">
-        <v>0.00056775822670771</v>
+        <v>0.002825625173998755</v>
       </c>
       <c r="J6" t="n">
-        <v>0.001265812514272724</v>
+        <v>0.003543583376273183</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0009167842968174325</v>
+        <v>0.003184611500800672</v>
       </c>
       <c r="L6" t="n">
-        <v>0.008268321424232379</v>
+        <v>0.004721933152998506</v>
       </c>
       <c r="M6" t="n">
-        <v>0.02090929434356055</v>
+        <v>0.03102526593065996</v>
       </c>
       <c r="N6" t="n">
-        <v>1.000521178736806</v>
+        <v>1.000651724158776</v>
       </c>
       <c r="O6" t="n">
-        <v>0.02100587358425596</v>
+        <v>0.03127446885712171</v>
       </c>
       <c r="P6" t="n">
-        <v>1181.47024605372</v>
+        <v>1179.891813505729</v>
       </c>
       <c r="Q6" t="n">
-        <v>3154.630867659759</v>
+        <v>2833.444165258441</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_5</t>
+          <t>model_26_9_19</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9991457600061304</v>
+        <v>0.9976424503088017</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7893179398893702</v>
+        <v>0.6709585797988461</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9986252912654667</v>
+        <v>0.9955499156627761</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9977474017452757</v>
+        <v>0.982435808269581</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9981503031033563</v>
+        <v>0.9930077599437028</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0004248646641894825</v>
+        <v>0.0009503259656209959</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1250699718727855</v>
+        <v>0.1953332008806542</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0006085452721374034</v>
+        <v>0.002784778566361065</v>
       </c>
       <c r="J7" t="n">
-        <v>0.001334548865570692</v>
+        <v>0.003499967252673531</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0009715492215509819</v>
+        <v>0.003142370479224665</v>
       </c>
       <c r="L7" t="n">
-        <v>0.008131576566168567</v>
+        <v>0.004725410565675619</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0206122454911997</v>
+        <v>0.03082735742195552</v>
       </c>
       <c r="N7" t="n">
-        <v>1.000506475624781</v>
+        <v>1.000643436051091</v>
       </c>
       <c r="O7" t="n">
-        <v>0.0207074526744675</v>
+        <v>0.03107497069630434</v>
       </c>
       <c r="P7" t="n">
-        <v>1181.527479753906</v>
+        <v>1179.917411021032</v>
       </c>
       <c r="Q7" t="n">
-        <v>3154.688101359945</v>
+        <v>2833.469762773744</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_6</t>
+          <t>model_26_9_18</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9991687204700386</v>
+        <v>0.9976772165361729</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7885305606341055</v>
+        <v>0.6707734207018483</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9984251539394492</v>
+        <v>0.9956236854125367</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9977658279599153</v>
+        <v>0.9826910200937821</v>
       </c>
       <c r="F8" t="n">
-        <v>0.99807636666504</v>
+        <v>0.9931156913971628</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0004134450516005154</v>
+        <v>0.0009363117335049415</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1255373942117234</v>
+        <v>0.1954431193190886</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0006971404926860736</v>
+        <v>0.002738614852954408</v>
       </c>
       <c r="J8" t="n">
-        <v>0.001323632279005574</v>
+        <v>0.003449111907838505</v>
       </c>
       <c r="K8" t="n">
-        <v>0.001010384172953444</v>
+        <v>0.003093865191877297</v>
       </c>
       <c r="L8" t="n">
-        <v>0.008023234686514136</v>
+        <v>0.00472812256597563</v>
       </c>
       <c r="M8" t="n">
-        <v>0.02033334826339517</v>
+        <v>0.03059921132161647</v>
       </c>
       <c r="N8" t="n">
-        <v>1.000492862453556</v>
+        <v>1.000633947451918</v>
       </c>
       <c r="O8" t="n">
-        <v>0.02042726723090346</v>
+        <v>0.03084499206772871</v>
       </c>
       <c r="P8" t="n">
-        <v>1181.581971876848</v>
+        <v>1179.947124176637</v>
       </c>
       <c r="Q8" t="n">
-        <v>3154.742593482886</v>
+        <v>2833.499475929349</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_7</t>
+          <t>model_26_9_17</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9991422551287971</v>
+        <v>0.9977153222114611</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7870767108021173</v>
+        <v>0.6705623074267818</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9982250971970668</v>
+        <v>0.9957045985630982</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9976443415315698</v>
+        <v>0.9829733105684954</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9979235451618998</v>
+        <v>0.9932346000026666</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0004266078494090137</v>
+        <v>0.0009209513732125989</v>
       </c>
       <c r="H9" t="n">
-        <v>0.1264004622750343</v>
+        <v>0.1955684452787868</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0007857000411037267</v>
+        <v>0.002687980934505769</v>
       </c>
       <c r="J9" t="n">
-        <v>0.001395606753278005</v>
+        <v>0.003392860676218941</v>
       </c>
       <c r="K9" t="n">
-        <v>0.001090653330933577</v>
+        <v>0.003040426681664194</v>
       </c>
       <c r="L9" t="n">
-        <v>0.008387944628652366</v>
+        <v>0.004730785327554941</v>
       </c>
       <c r="M9" t="n">
-        <v>0.02065448739158185</v>
+        <v>0.03034718064685085</v>
       </c>
       <c r="N9" t="n">
-        <v>1.000508553653145</v>
+        <v>1.00062354743137</v>
       </c>
       <c r="O9" t="n">
-        <v>0.02074988968859176</v>
+        <v>0.03059093701767329</v>
       </c>
       <c r="P9" t="n">
-        <v>1181.519290704338</v>
+        <v>1179.980206641835</v>
       </c>
       <c r="Q9" t="n">
-        <v>3154.679912310376</v>
+        <v>2833.532558394547</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_8</t>
+          <t>model_26_9_16</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9991387841487958</v>
+        <v>0.9977595861091405</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7855804437305456</v>
+        <v>0.6703297350277386</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9979918754094526</v>
+        <v>0.9957957754528541</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9976192765451187</v>
+        <v>0.9833116777892161</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9978111300394102</v>
+        <v>0.9933731260102349</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0004283341754570126</v>
+        <v>0.0009031086395211981</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1272887110440912</v>
+        <v>0.1957065103014633</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0008889408314229968</v>
+        <v>0.002630924162296774</v>
       </c>
       <c r="J10" t="n">
-        <v>0.001410456471448396</v>
+        <v>0.003325435188608842</v>
       </c>
       <c r="K10" t="n">
-        <v>0.001149699126460124</v>
+        <v>0.00297817194880567</v>
       </c>
       <c r="L10" t="n">
-        <v>0.008441815630424608</v>
+        <v>0.004732127632102942</v>
       </c>
       <c r="M10" t="n">
-        <v>0.02069623577989516</v>
+        <v>0.03005176599671304</v>
       </c>
       <c r="N10" t="n">
-        <v>1.000510611583911</v>
+        <v>1.00061146667327</v>
       </c>
       <c r="O10" t="n">
-        <v>0.02079183091113359</v>
+        <v>0.030293149520982</v>
       </c>
       <c r="P10" t="n">
-        <v>1181.511213766515</v>
+        <v>1180.019335404473</v>
       </c>
       <c r="Q10" t="n">
-        <v>3154.671835372554</v>
+        <v>2833.571687157185</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_9</t>
+          <t>model_26_9_15</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9991514016535703</v>
+        <v>0.9978062115700133</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7848278170738933</v>
+        <v>0.6700643227973577</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9979534695168992</v>
+        <v>0.9958919302905807</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9975517504460207</v>
+        <v>0.9836735635044036</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9977568602037765</v>
+        <v>0.9935202792060389</v>
       </c>
       <c r="G11" t="n">
-        <v>0.000422058735337814</v>
+        <v>0.0008843139620253907</v>
       </c>
       <c r="H11" t="n">
-        <v>0.1277355027392588</v>
+        <v>0.1958640704666288</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0009059420504801591</v>
+        <v>0.002570752284448824</v>
       </c>
       <c r="J11" t="n">
-        <v>0.001450462219814162</v>
+        <v>0.003253323236530066</v>
       </c>
       <c r="K11" t="n">
-        <v>0.001178204238113494</v>
+        <v>0.002912040086241603</v>
       </c>
       <c r="L11" t="n">
-        <v>0.008231137748371311</v>
+        <v>0.004734289055704243</v>
       </c>
       <c r="M11" t="n">
-        <v>0.02054406813018819</v>
+        <v>0.02973741686874283</v>
       </c>
       <c r="N11" t="n">
-        <v>1.000503130713594</v>
+        <v>1.00059874138373</v>
       </c>
       <c r="O11" t="n">
-        <v>0.02063896040480096</v>
+        <v>0.02997627545985583</v>
       </c>
       <c r="P11" t="n">
-        <v>1181.540732140697</v>
+        <v>1180.061396795438</v>
       </c>
       <c r="Q11" t="n">
-        <v>3154.701353746736</v>
+        <v>2833.61374854815</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_10</t>
+          <t>model_26_9_14</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.9991532415378691</v>
+        <v>0.997859006336132</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7842017835392585</v>
+        <v>0.6697643456087748</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9978966007087859</v>
+        <v>0.9959997195865378</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9974688781143694</v>
+        <v>0.9840903579374524</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9976861596792745</v>
+        <v>0.993687728384444</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0004211436507826964</v>
+        <v>0.000863032443642609</v>
       </c>
       <c r="H12" t="n">
-        <v>0.1281071432886585</v>
+        <v>0.1960421498841114</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0009311162880768342</v>
+        <v>0.002503299782806605</v>
       </c>
       <c r="J12" t="n">
-        <v>0.001499559823419508</v>
+        <v>0.003170269778155372</v>
       </c>
       <c r="K12" t="n">
-        <v>0.00121533953291114</v>
+        <v>0.002836787041329812</v>
       </c>
       <c r="L12" t="n">
-        <v>0.00802514181685853</v>
+        <v>0.004734775369115369</v>
       </c>
       <c r="M12" t="n">
-        <v>0.02052178478550773</v>
+        <v>0.02937741383516611</v>
       </c>
       <c r="N12" t="n">
-        <v>1.000502039853231</v>
+        <v>1.000584332331842</v>
       </c>
       <c r="O12" t="n">
-        <v>0.02061657413419321</v>
+        <v>0.02961338078919523</v>
       </c>
       <c r="P12" t="n">
-        <v>1181.545073138443</v>
+        <v>1180.110116547127</v>
       </c>
       <c r="Q12" t="n">
-        <v>3154.705694744481</v>
+        <v>2833.662468299839</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_11</t>
+          <t>model_26_9_13</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9991531220676136</v>
+        <v>0.9979159433091874</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7836224209326448</v>
+        <v>0.669419041080241</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9978514992790321</v>
+        <v>0.996117412979891</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9973917051114765</v>
+        <v>0.9845425867811534</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9976236330389574</v>
+        <v>0.993869918677271</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0004212030704894943</v>
+        <v>0.0008400812057109638</v>
       </c>
       <c r="H13" t="n">
-        <v>0.1284510779591059</v>
+        <v>0.196247137568628</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0009510814349867998</v>
+        <v>0.002429649484435632</v>
       </c>
       <c r="J13" t="n">
-        <v>0.001545280867217452</v>
+        <v>0.00308015540409473</v>
       </c>
       <c r="K13" t="n">
-        <v>0.00124818151304126</v>
+        <v>0.002754909217746575</v>
       </c>
       <c r="L13" t="n">
-        <v>0.007857430720055625</v>
+        <v>0.004734816247618888</v>
       </c>
       <c r="M13" t="n">
-        <v>0.02052323245713244</v>
+        <v>0.02898415439013123</v>
       </c>
       <c r="N13" t="n">
-        <v>1.000502110686688</v>
+        <v>1.00056879276496</v>
       </c>
       <c r="O13" t="n">
-        <v>0.02061802849255846</v>
+        <v>0.02921696258301451</v>
       </c>
       <c r="P13" t="n">
-        <v>1181.54479097574</v>
+        <v>1180.164023994668</v>
       </c>
       <c r="Q13" t="n">
-        <v>3154.705412581779</v>
+        <v>2833.71637574738</v>
       </c>
     </row>
     <row r="14">
@@ -1182,712 +1182,712 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.9991453835155425</v>
+        <v>0.997982505668534</v>
       </c>
       <c r="C14" t="n">
-        <v>0.782742343471599</v>
+        <v>0.6690360496881356</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9977911164040296</v>
+        <v>0.9962511106226944</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9973074503110002</v>
+        <v>0.9850867022146867</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9975506680778284</v>
+        <v>0.9940836682807568</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0004250519154869289</v>
+        <v>0.0008132499840165691</v>
       </c>
       <c r="H14" t="n">
-        <v>0.1289735299573495</v>
+        <v>0.1964744978033484</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0009778112521311591</v>
+        <v>0.002345984029617712</v>
       </c>
       <c r="J14" t="n">
-        <v>0.001595197512655051</v>
+        <v>0.002971731046841627</v>
       </c>
       <c r="K14" t="n">
-        <v>0.001286506198190435</v>
+        <v>0.002658848379083785</v>
       </c>
       <c r="L14" t="n">
-        <v>0.007711417925054255</v>
+        <v>0.004730843814423458</v>
       </c>
       <c r="M14" t="n">
-        <v>0.02061678722514565</v>
+        <v>0.02851753818295978</v>
       </c>
       <c r="N14" t="n">
-        <v>1.00050669884461</v>
+        <v>1.000550626182169</v>
       </c>
       <c r="O14" t="n">
-        <v>0.02071201538651097</v>
+        <v>0.02874659839429081</v>
       </c>
       <c r="P14" t="n">
-        <v>1181.526598484826</v>
+        <v>1180.228944024529</v>
       </c>
       <c r="Q14" t="n">
-        <v>3154.687220090865</v>
+        <v>2833.781295777241</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_13</t>
+          <t>model_26_9_11</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9991391452629971</v>
+        <v>0.9980584223544827</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7821757066820803</v>
+        <v>0.6685721883210836</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9977529469423364</v>
+        <v>0.9964003230745442</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9972261467582721</v>
+        <v>0.9857244076393253</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9974887298153751</v>
+        <v>0.9943288991926137</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0004281545717566954</v>
+        <v>0.0007826480424539799</v>
       </c>
       <c r="H15" t="n">
-        <v>0.1293099100330426</v>
+        <v>0.1967498659485983</v>
       </c>
       <c r="I15" t="n">
-        <v>0.000994707809830917</v>
+        <v>0.002252609700895514</v>
       </c>
       <c r="J15" t="n">
-        <v>0.001643365695256006</v>
+        <v>0.002844657274399132</v>
       </c>
       <c r="K15" t="n">
-        <v>0.001319039134143364</v>
+        <v>0.002548639580214189</v>
       </c>
       <c r="L15" t="n">
-        <v>0.007591695450699924</v>
+        <v>0.00472205732615566</v>
       </c>
       <c r="M15" t="n">
-        <v>0.02069189628228151</v>
+        <v>0.02797584748410636</v>
       </c>
       <c r="N15" t="n">
-        <v>1.000510397480682</v>
+        <v>1.000529906562641</v>
       </c>
       <c r="O15" t="n">
-        <v>0.02078747136954439</v>
+        <v>0.02820055669623263</v>
       </c>
       <c r="P15" t="n">
-        <v>1181.512052557234</v>
+        <v>1180.30565492362</v>
       </c>
       <c r="Q15" t="n">
-        <v>3154.672674163272</v>
+        <v>2833.858006676332</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_14</t>
+          <t>model_26_9_10</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.9991321247940257</v>
+        <v>0.9981412037852979</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7816979267958027</v>
+        <v>0.6680417155851922</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9977148316555817</v>
+        <v>0.9965639484545433</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9971553525701291</v>
+        <v>0.9864286791316127</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9974327464638982</v>
+        <v>0.9945989586232206</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0004316462710606053</v>
+        <v>0.0007492789289762485</v>
       </c>
       <c r="H16" t="n">
-        <v>0.1295935408125533</v>
+        <v>0.1970647774798524</v>
       </c>
       <c r="I16" t="n">
-        <v>0.00101158038579414</v>
+        <v>0.002150216034482764</v>
       </c>
       <c r="J16" t="n">
-        <v>0.001685307618666933</v>
+        <v>0.002704319068244827</v>
       </c>
       <c r="K16" t="n">
-        <v>0.00134844426621974</v>
+        <v>0.002427272639785521</v>
       </c>
       <c r="L16" t="n">
-        <v>0.007481214045248123</v>
+        <v>0.004708527868121364</v>
       </c>
       <c r="M16" t="n">
-        <v>0.02077609855243773</v>
+        <v>0.02737295981395232</v>
       </c>
       <c r="N16" t="n">
-        <v>1.000514559889881</v>
+        <v>1.000507313377375</v>
       </c>
       <c r="O16" t="n">
-        <v>0.02087206256680561</v>
+        <v>0.02759282647703918</v>
       </c>
       <c r="P16" t="n">
-        <v>1181.495808244247</v>
+        <v>1180.392798483868</v>
       </c>
       <c r="Q16" t="n">
-        <v>3154.656429850285</v>
+        <v>2833.94515023658</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_15</t>
+          <t>model_26_9_9</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.9991284968640066</v>
+        <v>0.9982313656914039</v>
       </c>
       <c r="C17" t="n">
-        <v>0.7812461137781166</v>
+        <v>0.6674287491262394</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9976904613240342</v>
+        <v>0.9967381400204455</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9971053442097882</v>
+        <v>0.9872228081053046</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9973942804600003</v>
+        <v>0.9948963041037656</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0004334506577438871</v>
+        <v>0.0007129347531557891</v>
       </c>
       <c r="H17" t="n">
-        <v>0.129861756537158</v>
+        <v>0.1974286608486591</v>
       </c>
       <c r="I17" t="n">
-        <v>0.001022368452874219</v>
+        <v>0.002041210248882864</v>
       </c>
       <c r="J17" t="n">
-        <v>0.00171493500580618</v>
+        <v>0.002546075213646777</v>
       </c>
       <c r="K17" t="n">
-        <v>0.001368648450057135</v>
+        <v>0.002293643122967967</v>
       </c>
       <c r="L17" t="n">
-        <v>0.007355298258486441</v>
+        <v>0.004695535028056486</v>
       </c>
       <c r="M17" t="n">
-        <v>0.02081947784513068</v>
+        <v>0.0267008380609259</v>
       </c>
       <c r="N17" t="n">
-        <v>1.000516710875712</v>
+        <v>1.00048270587025</v>
       </c>
       <c r="O17" t="n">
-        <v>0.02091564222681279</v>
+        <v>0.02691530606898859</v>
       </c>
       <c r="P17" t="n">
-        <v>1181.487465182378</v>
+        <v>1180.492241304075</v>
       </c>
       <c r="Q17" t="n">
-        <v>3154.648086788416</v>
+        <v>2834.044593056787</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_16</t>
+          <t>model_26_9_8</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.9991216021913993</v>
+        <v>0.998330734434299</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7809132311259882</v>
+        <v>0.6667061830821097</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9976599869104191</v>
+        <v>0.9969265991643285</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9970499368892969</v>
+        <v>0.9881256664747323</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9973501838336802</v>
+        <v>0.9952276852544737</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0004368797909886772</v>
+        <v>0.0006728793104659488</v>
       </c>
       <c r="H18" t="n">
-        <v>0.1300593700592432</v>
+        <v>0.1978576072656823</v>
       </c>
       <c r="I18" t="n">
-        <v>0.001035858627091304</v>
+        <v>0.001923276082977222</v>
       </c>
       <c r="J18" t="n">
-        <v>0.001747760999767172</v>
+        <v>0.002366165157135224</v>
       </c>
       <c r="K18" t="n">
-        <v>0.001391810105921962</v>
+        <v>0.002144717694639885</v>
       </c>
       <c r="L18" t="n">
-        <v>0.007259219300265425</v>
+        <v>0.004676633383263123</v>
       </c>
       <c r="M18" t="n">
-        <v>0.02090166957419137</v>
+        <v>0.02593991731802453</v>
       </c>
       <c r="N18" t="n">
-        <v>1.000520798700728</v>
+        <v>1.000455585580159</v>
       </c>
       <c r="O18" t="n">
-        <v>0.0209982135963651</v>
+        <v>0.02614827341470634</v>
       </c>
       <c r="P18" t="n">
-        <v>1181.471704957077</v>
+        <v>1180.607889150122</v>
       </c>
       <c r="Q18" t="n">
-        <v>3154.632326563116</v>
+        <v>2834.160240902834</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_17</t>
+          <t>model_26_9_7</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.9991149278833793</v>
+        <v>0.9984451527691709</v>
       </c>
       <c r="C19" t="n">
-        <v>0.7806355193993573</v>
+        <v>0.6658769603814604</v>
       </c>
       <c r="D19" t="n">
-        <v>0.9976443860521447</v>
+        <v>0.9971382025599234</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9969920581731668</v>
+        <v>0.9891935514566719</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9973109664278536</v>
+        <v>0.9956117419667141</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0004401993237382321</v>
+        <v>0.0006267573920275544</v>
       </c>
       <c r="H19" t="n">
-        <v>0.1302242317366932</v>
+        <v>0.1983498696813433</v>
       </c>
       <c r="I19" t="n">
-        <v>0.001042764692576828</v>
+        <v>0.00179085868232419</v>
       </c>
       <c r="J19" t="n">
-        <v>0.001782051168815341</v>
+        <v>0.002153370710127606</v>
       </c>
       <c r="K19" t="n">
-        <v>0.001412408961967647</v>
+        <v>0.001972119433542498</v>
       </c>
       <c r="L19" t="n">
-        <v>0.007162909487443266</v>
+        <v>0.004643888758097825</v>
       </c>
       <c r="M19" t="n">
-        <v>0.02098092761863098</v>
+        <v>0.02503512316781275</v>
       </c>
       <c r="N19" t="n">
-        <v>1.000524755872423</v>
+        <v>1.000424357868676</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0210778377307179</v>
+        <v>0.02523621172485179</v>
       </c>
       <c r="P19" t="n">
-        <v>1181.456565850267</v>
+        <v>1180.74990205355</v>
       </c>
       <c r="Q19" t="n">
-        <v>3154.617187456305</v>
+        <v>2834.302253806262</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_18</t>
+          <t>model_26_9_6</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.9991067707855492</v>
+        <v>0.9985712455960988</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7803414999584553</v>
+        <v>0.6648915899405275</v>
       </c>
       <c r="D20" t="n">
-        <v>0.9976158070684163</v>
+        <v>0.9973690516320017</v>
       </c>
       <c r="E20" t="n">
-        <v>0.9969418125301216</v>
+        <v>0.9904007114271541</v>
       </c>
       <c r="F20" t="n">
-        <v>0.9972705857516765</v>
+        <v>0.9960401093065364</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0004442563365861555</v>
+        <v>0.0005759294973047023</v>
       </c>
       <c r="H20" t="n">
-        <v>0.1303987743777912</v>
+        <v>0.1989348281408677</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0010554158127694</v>
+        <v>0.001646397701526423</v>
       </c>
       <c r="J20" t="n">
-        <v>0.00181181913377986</v>
+        <v>0.001912823326548944</v>
       </c>
       <c r="K20" t="n">
-        <v>0.001433618823203185</v>
+        <v>0.001779607610137752</v>
       </c>
       <c r="L20" t="n">
-        <v>0.007086090072741452</v>
+        <v>0.004594761424558987</v>
       </c>
       <c r="M20" t="n">
-        <v>0.02107738922604399</v>
+        <v>0.02399853114889956</v>
       </c>
       <c r="N20" t="n">
-        <v>1.000529592184524</v>
+        <v>1.000389943887528</v>
       </c>
       <c r="O20" t="n">
-        <v>0.02117474489065159</v>
+        <v>0.02419129353187011</v>
       </c>
       <c r="P20" t="n">
-        <v>1181.438217654944</v>
+        <v>1180.919050610545</v>
       </c>
       <c r="Q20" t="n">
-        <v>3154.598839260983</v>
+        <v>2834.471402363257</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_19</t>
+          <t>model_26_9_5</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.9990991464294744</v>
+        <v>0.9987030318834146</v>
       </c>
       <c r="C21" t="n">
-        <v>0.7800650014087551</v>
+        <v>0.6637321856160763</v>
       </c>
       <c r="D21" t="n">
-        <v>0.9975905859491682</v>
+        <v>0.9976135116026333</v>
       </c>
       <c r="E21" t="n">
-        <v>0.996896962830458</v>
+        <v>0.9916941794242169</v>
       </c>
       <c r="F21" t="n">
-        <v>0.9972346671872551</v>
+        <v>0.9964970610966682</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0004480483850814688</v>
+        <v>0.0005228065742899436</v>
       </c>
       <c r="H21" t="n">
-        <v>0.1305629158610086</v>
+        <v>0.1996231006315209</v>
       </c>
       <c r="I21" t="n">
-        <v>0.001066580499870709</v>
+        <v>0.001493419277982022</v>
       </c>
       <c r="J21" t="n">
-        <v>0.00183839027920349</v>
+        <v>0.001655077584439994</v>
       </c>
       <c r="K21" t="n">
-        <v>0.001452484970065468</v>
+        <v>0.001574249698484545</v>
       </c>
       <c r="L21" t="n">
-        <v>0.007013981776369402</v>
+        <v>0.004528532791504232</v>
       </c>
       <c r="M21" t="n">
-        <v>0.02116715344777065</v>
+        <v>0.02286496390309732</v>
       </c>
       <c r="N21" t="n">
-        <v>1.000534112636077</v>
+        <v>1.000353976014352</v>
       </c>
       <c r="O21" t="n">
-        <v>0.02126492372992743</v>
+        <v>0.0230486211820012</v>
       </c>
       <c r="P21" t="n">
-        <v>1181.421218657934</v>
+        <v>1181.112598002281</v>
       </c>
       <c r="Q21" t="n">
-        <v>3154.581840263973</v>
+        <v>2834.664949754992</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_20</t>
+          <t>model_26_9_4</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.9990887859353936</v>
+        <v>0.9988350583255881</v>
       </c>
       <c r="C22" t="n">
-        <v>0.7798400036233434</v>
+        <v>0.6623626221371663</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9975705254073898</v>
+        <v>0.9978477854560971</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9968368783312157</v>
+        <v>0.9930856100188789</v>
       </c>
       <c r="F22" t="n">
-        <v>0.9971923200615118</v>
+        <v>0.9969686679419353</v>
       </c>
       <c r="G22" t="n">
-        <v>0.000453201278729685</v>
+        <v>0.0004695868450878726</v>
       </c>
       <c r="H22" t="n">
-        <v>0.1306964842658273</v>
+        <v>0.2004361326746636</v>
       </c>
       <c r="I22" t="n">
-        <v>0.001075460743044468</v>
+        <v>0.001346815133802643</v>
       </c>
       <c r="J22" t="n">
-        <v>0.001873987261547765</v>
+        <v>0.001377811110102284</v>
       </c>
       <c r="K22" t="n">
-        <v>0.001474727704605079</v>
+        <v>0.001362305683914716</v>
       </c>
       <c r="L22" t="n">
-        <v>0.006951163868558534</v>
+        <v>0.004438765344917176</v>
       </c>
       <c r="M22" t="n">
-        <v>0.02128852457850672</v>
+        <v>0.02166995258619346</v>
       </c>
       <c r="N22" t="n">
-        <v>1.000540255333387</v>
+        <v>1.000317942596728</v>
       </c>
       <c r="O22" t="n">
-        <v>0.02138685546933141</v>
+        <v>0.02184401122642675</v>
       </c>
       <c r="P22" t="n">
-        <v>1181.398348414515</v>
+        <v>1181.327314605717</v>
       </c>
       <c r="Q22" t="n">
-        <v>3154.558970020553</v>
+        <v>2834.879666358428</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_21</t>
+          <t>model_26_9_3</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.9990807669774415</v>
+        <v>0.9989689466018259</v>
       </c>
       <c r="C23" t="n">
-        <v>0.7796236573546117</v>
+        <v>0.6607327506967184</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9975481991445183</v>
+        <v>0.9980874386808062</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9967949601908598</v>
+        <v>0.9945607585762859</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9971592757890444</v>
+        <v>0.9974625380685743</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0004571895863503656</v>
+        <v>0.000415616612402575</v>
       </c>
       <c r="H23" t="n">
-        <v>0.1308249167566186</v>
+        <v>0.2014036947684938</v>
       </c>
       <c r="I23" t="n">
-        <v>0.001085343957847453</v>
+        <v>0.001196844680895394</v>
       </c>
       <c r="J23" t="n">
-        <v>0.001898821608525344</v>
+        <v>0.00108386239199466</v>
       </c>
       <c r="K23" t="n">
-        <v>0.001492084135948354</v>
+        <v>0.001140356366667842</v>
       </c>
       <c r="L23" t="n">
-        <v>0.006894561267170213</v>
+        <v>0.004312282202522755</v>
       </c>
       <c r="M23" t="n">
-        <v>0.02138199210434719</v>
+        <v>0.02038667732619946</v>
       </c>
       <c r="N23" t="n">
-        <v>1.000545009742883</v>
+        <v>1.00028140103662</v>
       </c>
       <c r="O23" t="n">
-        <v>0.02148075471814287</v>
+        <v>0.02055042836903902</v>
       </c>
       <c r="P23" t="n">
-        <v>1181.380824806629</v>
+        <v>1181.571494654887</v>
       </c>
       <c r="Q23" t="n">
-        <v>3154.541446412667</v>
+        <v>2835.123846407598</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_22</t>
+          <t>model_26_9_2</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.9990744880969278</v>
+        <v>0.9990951044454108</v>
       </c>
       <c r="C24" t="n">
-        <v>0.7794283675583685</v>
+        <v>0.6588596541671699</v>
       </c>
       <c r="D24" t="n">
-        <v>0.9975312315400181</v>
+        <v>0.9983211425179247</v>
       </c>
       <c r="E24" t="n">
-        <v>0.9967612719181099</v>
+        <v>0.9960420823072649</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9971331325664402</v>
+        <v>0.9979536669418103</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0004603124493398466</v>
+        <v>0.0003647625095291208</v>
       </c>
       <c r="H24" t="n">
-        <v>0.1309408492157485</v>
+        <v>0.2025156457819907</v>
       </c>
       <c r="I24" t="n">
-        <v>0.001092855043824225</v>
+        <v>0.001050597242158066</v>
       </c>
       <c r="J24" t="n">
-        <v>0.001918780181292126</v>
+        <v>0.0007886831643587288</v>
       </c>
       <c r="K24" t="n">
-        <v>0.001505815806048473</v>
+        <v>0.0009196389913595135</v>
       </c>
       <c r="L24" t="n">
-        <v>0.006833430271503621</v>
+        <v>0.004154183685129559</v>
       </c>
       <c r="M24" t="n">
-        <v>0.02145489336584656</v>
+        <v>0.01909875675349369</v>
       </c>
       <c r="N24" t="n">
-        <v>1.000548732467122</v>
+        <v>1.00024696931075</v>
       </c>
       <c r="O24" t="n">
-        <v>0.02155399270781515</v>
+        <v>0.01925216288659143</v>
       </c>
       <c r="P24" t="n">
-        <v>1181.367210122727</v>
+        <v>1181.832528149953</v>
       </c>
       <c r="Q24" t="n">
-        <v>3154.527831728765</v>
+        <v>2835.384879902665</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_23</t>
+          <t>model_26_9_1</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.9990539039467419</v>
+        <v>0.9992028092581945</v>
       </c>
       <c r="C25" t="n">
-        <v>0.7791694860849299</v>
+        <v>0.6567678479050425</v>
       </c>
       <c r="D25" t="n">
-        <v>0.9975080161014293</v>
+        <v>0.9985403114811828</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9966473662025999</v>
+        <v>0.9974358060318398</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9970591077276789</v>
+        <v>0.9984152448504306</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0004705501789229811</v>
+        <v>0.0003213468052524113</v>
       </c>
       <c r="H25" t="n">
-        <v>0.131094532441479</v>
+        <v>0.2037574323405151</v>
       </c>
       <c r="I25" t="n">
-        <v>0.001103131871954403</v>
+        <v>0.0009134454524296129</v>
       </c>
       <c r="J25" t="n">
-        <v>0.001986263472241719</v>
+        <v>0.0005109597444510161</v>
       </c>
       <c r="K25" t="n">
-        <v>0.001544697189590013</v>
+        <v>0.0007122020638180409</v>
       </c>
       <c r="L25" t="n">
-        <v>0.006742524367523114</v>
+        <v>0.003933210779947714</v>
       </c>
       <c r="M25" t="n">
-        <v>0.0216921686081171</v>
+        <v>0.01792614864527267</v>
       </c>
       <c r="N25" t="n">
-        <v>1.00056093673103</v>
+        <v>1.000217573892414</v>
       </c>
       <c r="O25" t="n">
-        <v>0.02179236391546635</v>
+        <v>0.01807013608804188</v>
       </c>
       <c r="P25" t="n">
-        <v>1181.323215908835</v>
+        <v>1182.085979255683</v>
       </c>
       <c r="Q25" t="n">
-        <v>3154.483837514873</v>
+        <v>2835.638331008394</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>model_26_9_24</t>
+          <t>model_26_9_0</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.999048156710744</v>
+        <v>0.9992672939283358</v>
       </c>
       <c r="C26" t="n">
-        <v>0.7789821296684627</v>
+        <v>0.6544395980212336</v>
       </c>
       <c r="D26" t="n">
-        <v>0.997485674404342</v>
+        <v>0.9987042288268448</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9966260764200761</v>
+        <v>0.998582808586285</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9970376888503837</v>
+        <v>0.9987836603809076</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0004734086232826511</v>
+        <v>0.0002953530980366107</v>
       </c>
       <c r="H26" t="n">
-        <v>0.1312057553036697</v>
+        <v>0.2051395820467021</v>
       </c>
       <c r="I26" t="n">
-        <v>0.001113021919054887</v>
+        <v>0.0008108690794301227</v>
       </c>
       <c r="J26" t="n">
-        <v>0.001998876575823663</v>
+        <v>0.0002823997605413487</v>
       </c>
       <c r="K26" t="n">
-        <v>0.001555947407720539</v>
+        <v>0.0005466330790953092</v>
       </c>
       <c r="L26" t="n">
-        <v>0.006702913108868424</v>
+        <v>0.003668562820852012</v>
       </c>
       <c r="M26" t="n">
-        <v>0.02175795540216615</v>
+        <v>0.01718584004454279</v>
       </c>
       <c r="N26" t="n">
-        <v>1.000564344245269</v>
+        <v>1.000199974364537</v>
       </c>
       <c r="O26" t="n">
-        <v>0.02185845457623192</v>
+        <v>0.01732388113796566</v>
       </c>
       <c r="P26" t="n">
-        <v>1181.311103290826</v>
+        <v>1182.254677949784</v>
       </c>
       <c r="Q26" t="n">
-        <v>3154.471724896865</v>
+        <v>2835.807029702496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>